<commit_message>
Ajout de Orga travail
</commit_message>
<xml_diff>
--- a/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
+++ b/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\Node\Cahier des charges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA70B1F-B2FF-4A6C-9E2F-7DFCB9980460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77789E7-F507-407F-9F38-80D0BABE52FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{1E56176C-5C6E-4D46-B358-12925D1648B7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="対応中" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">対応中!$C$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">対応中!$C$1:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="120">
   <si>
     <t>No.</t>
   </si>
@@ -183,10 +183,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Creer le generateur de model une fois L7apprentissage termine</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>Objectif Aujourd'hui</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -195,6 +191,320 @@
 - Finir la lecture de Express Mozilla
 - Apprendre jade et EJS" 
 - Faire les cours udemy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今日</t>
+    <rPh sb="0" eb="2">
+      <t>キョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Creer le generateur de model une fois L'apprentissage termine</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>1) Apprendre a utiliser git ignore
+2) Apprendre a utiliser le Async
+3) Gerrer le proxy
+4) le commit modif
+5) rendre beau le code 
+6) Apprendre comment utiliser les quelques fonctions que je connais pas dans git
+7) Faire en sorte que le check de diagnosis est bie nfait</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>views</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>newUser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>updateUser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deleteUser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>searchUser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>adminConnection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>collection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Users</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>naem</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>first name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inscription date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>country</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>job</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>salary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UsersDetail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Users Details</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>viewDetailsUser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Model</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UOW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>The hostname of the database. Default is localhost.</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>The port number to connect to. Default is 3306.</t>
+  </si>
+  <si>
+    <t>localAddress</t>
+  </si>
+  <si>
+    <t>The source IP address to use for TCP connection. (Optional)</t>
+  </si>
+  <si>
+    <t>socketPath</t>
+  </si>
+  <si>
+    <t>The path to a unix domain socket to connect to. When used host and port are ignored.</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>The MySQL user to authenticate as.</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>The password of that MySQL user.</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>Name of the database to use for this connection (Optional).</t>
+  </si>
+  <si>
+    <t>charset</t>
+  </si>
+  <si>
+    <t>The charset for the connection. This is called "collation" in the SQL-level of MySQL (like utf8_general_ci). If a SQL-level charset is specified (like utf8mb4) then the default collation for that charset is used. (Default: 'UTF8_GENERAL_CI')</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>The timezone used to store local dates. Default is : 'local'.</t>
+  </si>
+  <si>
+    <t>connectTimeout</t>
+  </si>
+  <si>
+    <t>The milliseconds before a timeout occurs during the initial connection to the MySQL server. (Default: 10 seconds)</t>
+  </si>
+  <si>
+    <t>stringifyObjects</t>
+  </si>
+  <si>
+    <t>Stringify objects instead of converting to values. See issue #501. (Default: 'false')</t>
+  </si>
+  <si>
+    <t>insecureAuth</t>
+  </si>
+  <si>
+    <t>Allow connecting to MySQL instances that ask for the old (insecure) authentication method. (Default: false)</t>
+  </si>
+  <si>
+    <t>typeCast</t>
+  </si>
+  <si>
+    <t>Determines if column values should be converted to native JavaScript types. (Default: true)</t>
+  </si>
+  <si>
+    <t>queryFormat</t>
+  </si>
+  <si>
+    <t>A custom query format function. See Custom format.</t>
+  </si>
+  <si>
+    <t>supportBigNumbers</t>
+  </si>
+  <si>
+    <t>When dealing with big numbers (BIGINT and DECIMAL columns) in the database, you should enable this option (Default: false).</t>
+  </si>
+  <si>
+    <t>bigNumberStrings</t>
+  </si>
+  <si>
+    <t>Enabling both supportBigNumbers and bigNumberStrings forces big numbers (BIGINT and DECIMAL columns) to be always returned as JavaScript String objects (Default: false).</t>
+  </si>
+  <si>
+    <t>Enabling supportBigNumbers but leaving bigNumberStrings disabled will return big numbers as String objects only when they cannot be accurately represented with JavaScript Number objects (which happens when they exceed the [-2^53, +2^53] range), otherwise they will be returned as Number objects. This option is ignored if supportBigNumbers is disabled.</t>
+  </si>
+  <si>
+    <t>dateStrings</t>
+  </si>
+  <si>
+    <t>Force date types (TIMESTAMP, DATETIME, DATE) to be returned as strings rather then inflated into JavaScript Date objects. (Default: false)</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>Prints protocol details to stdout. (Default: false)</t>
+  </si>
+  <si>
+    <t>trace</t>
+  </si>
+  <si>
+    <t>Generates stack traces on Error to include call site of library entrance ("long stack traces"). Slight performance penalty for most calls. Default is true.</t>
+  </si>
+  <si>
+    <t>multipleStatements</t>
+  </si>
+  <si>
+    <t>Allow multiple mysql statements per query. Be careful with this, it exposes you to SQL injection attacks. (Default: false)</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>List of connection flags to use other than the default ones. It is also possible to blacklist default ones. For more information, check Connection Flags.</t>
+  </si>
+  <si>
+    <t>ssl</t>
+  </si>
+  <si>
+    <t>object with ssl parameters or a string containing name of ssl profile. See SSL options.</t>
+  </si>
+  <si>
+    <t>nom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>prenom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parties</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>obj1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>nbr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>明日</t>
+    <rPh sb="0" eb="2">
+      <t>アシタ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>1) ok
+2) ok
+3) ok
+4) ok
+5) ok
+6) NON A faire ce soir ou dans le train
+7) A verif demain mais ca a l'air ok
+Ne pas oublier de changer le nom de check ou plutot donner une proposition</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1) Faire le 7)
+2) si 6 pas fait faire le 6
+3) Comprendre le doc de spice et voir un peu ce qu'est ce DCS
+4) Modif le code pour avoir juste les infos necessaires 
+5) Chercher pour check result le comment ca marche
+6) Finir le CRUD Mysql AU MOINS
+7) Si temps finir aussi le CRUD Mongo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8h</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -202,7 +512,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,8 +563,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +617,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -343,11 +687,146 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -358,9 +837,31 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -369,156 +870,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -532,6 +883,32 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -544,7 +921,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,102 +946,237 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{B9F7C401-71ED-4AD8-8EED-9CF337C7F41D}"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1223,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D38343-8F70-402C-9913-C6A4103E4390}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:R130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1243,7 +1755,9 @@
     <col min="10" max="10" width="8.875" style="9" customWidth="1"/>
     <col min="11" max="11" width="12.875" style="7" customWidth="1"/>
     <col min="12" max="12" width="19.875" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="7"/>
+    <col min="13" max="17" width="9" style="7"/>
+    <col min="18" max="18" width="62.25" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1281,40 +1795,40 @@
         <v>9</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:13" ht="276" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10">
+      <c r="A3" s="34">
         <f>COUNTA(G$3:G3)</f>
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="29" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="23">
@@ -1322,13 +1836,13 @@
       </c>
       <c r="I3" s="24" t="str">
         <f t="shared" ref="I3:I10" ca="1" si="0">IF(H3-NOW()&lt;=0,"遅れ",ROUNDDOWN(H3+1-NOW(),0)&amp;"j")</f>
-        <v>8j</v>
+        <v>5j</v>
       </c>
       <c r="J3" s="19">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="37"/>
+      <c r="L3" s="30"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
@@ -1342,13 +1856,13 @@
       <c r="C4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="26" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -1359,13 +1873,13 @@
       </c>
       <c r="I4" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8j</v>
+        <v>5j</v>
       </c>
       <c r="J4" s="16">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K4" s="11"/>
-      <c r="L4" s="38"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A5" s="10">
@@ -1378,14 +1892,14 @@
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="26" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>36</v>
+      <c r="F5" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>25</v>
@@ -1395,13 +1909,13 @@
       </c>
       <c r="I5" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29j</v>
+        <v>26j</v>
       </c>
       <c r="J5" s="16">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="K5" s="11"/>
-      <c r="L5" s="38"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
@@ -1414,13 +1928,13 @@
       <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="31"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
@@ -1429,13 +1943,13 @@
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29j</v>
+        <v>26j</v>
       </c>
       <c r="J6" s="16">
         <v>0</v>
       </c>
       <c r="K6" s="11"/>
-      <c r="L6" s="38"/>
+      <c r="L6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A7" s="10">
@@ -1448,13 +1962,13 @@
       <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="13" t="s">
         <v>11</v>
       </c>
@@ -1463,13 +1977,13 @@
       </c>
       <c r="I7" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29j</v>
+        <v>26j</v>
       </c>
       <c r="J7" s="16">
         <v>0</v>
       </c>
       <c r="K7" s="11"/>
-      <c r="L7" s="38"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A8" s="10">
@@ -1482,11 +1996,11 @@
       <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="27" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -1497,13 +2011,13 @@
       </c>
       <c r="I8" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>29j</v>
+        <v>26j</v>
       </c>
       <c r="J8" s="16">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="K8" s="11"/>
-      <c r="L8" s="38"/>
+      <c r="L8" s="31"/>
     </row>
     <row r="9" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A9" s="10">
@@ -1522,7 +2036,7 @@
       <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="27" t="s">
         <v>29</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -1533,15 +2047,15 @@
       </c>
       <c r="I9" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5j</v>
+        <v>2j</v>
       </c>
       <c r="J9" s="16">
         <v>0</v>
       </c>
       <c r="K9" s="11"/>
-      <c r="L9" s="38"/>
-    </row>
-    <row r="10" spans="1:13" ht="57" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A10" s="10">
         <f>COUNTA(G$3:G10)</f>
         <v>8</v>
@@ -1553,60 +2067,450 @@
         <v>12</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="14">
         <v>43661</v>
       </c>
-      <c r="I10" s="21" t="str">
+      <c r="I10" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>59j</v>
-      </c>
-      <c r="J10" s="22">
+        <v>56j</v>
+      </c>
+      <c r="J10" s="16">
         <v>0</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="39"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="J12" s="7"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="10">
+        <f>COUNTA(G$3:G11)</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="14">
+        <v>43605</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="31"/>
+    </row>
+    <row r="12" spans="1:13" ht="188.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="25">
+        <v>43606</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22">
+        <v>0</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="J13" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="G16" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="H17" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="H18" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="G22" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="E23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="F29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="H30" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="H31" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.4">
+      <c r="H32" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="H33" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="H34" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="E37" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F38" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="Q39" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="R39" s="50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="Q40" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="R40" s="48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="Q41" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="R41" s="44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q42" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="R42" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q43" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="R43" s="44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="Q44" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="R44" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q45" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="R45" s="44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q46" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="R46" s="44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" ht="60" x14ac:dyDescent="0.4">
+      <c r="Q47" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="R47" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18" x14ac:dyDescent="0.4">
+      <c r="Q48" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="R48" s="44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q49" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="R49" s="44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q50" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="R50" s="44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q51" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="R51" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q52" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="R52" s="44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q53" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="R53" s="44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q54" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="R54" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q55" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="R55" s="44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="17:18" ht="90" x14ac:dyDescent="0.4">
+      <c r="Q56" s="54"/>
+      <c r="R56" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q57" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="R57" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="17:18" x14ac:dyDescent="0.4">
+      <c r="Q58" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="R58" s="44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q59" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="R59" s="44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q60" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="R60" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q61" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="R61" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="17:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="Q62" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="R62" s="46" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="103" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J103" s="9">
         <v>1</v>
       </c>
     </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C125" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D126" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D127" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D128" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="129" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="E129" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="130" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="F130" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="1">
+  <autoFilter ref="C1:C12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="Q55:Q56"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="C1 C11:C1048576">
-    <cfRule type="expression" dxfId="28" priority="38">
+  <conditionalFormatting sqref="C1 C13:C124 C126:C1048576">
+    <cfRule type="expression" dxfId="39" priority="51">
       <formula>$C1="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="39">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>$C1="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="37" priority="53">
       <formula>$C1="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="41">
+    <cfRule type="expression" dxfId="36" priority="54">
       <formula>$C1="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -1619,13 +2523,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I2 I11:I1048576">
-    <cfRule type="expression" dxfId="24" priority="32">
+  <conditionalFormatting sqref="I1:I2 I24:I123 I13:I22 I125:I1048576">
+    <cfRule type="expression" dxfId="35" priority="45">
       <formula>$I1="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J11 J13:J1048576">
-    <cfRule type="dataBar" priority="42">
+  <conditionalFormatting sqref="J14:J1048576 J1:J12">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -1639,93 +2543,136 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="expression" dxfId="23" priority="28">
+    <cfRule type="expression" dxfId="34" priority="41">
       <formula>$C3="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="29">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>$C3="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="30">
+    <cfRule type="expression" dxfId="32" priority="43">
       <formula>$C3="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="31">
+    <cfRule type="expression" dxfId="31" priority="44">
       <formula>$C3="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I6">
-    <cfRule type="expression" dxfId="19" priority="27">
+    <cfRule type="expression" dxfId="30" priority="40">
       <formula>$I3="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I8">
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>$I7="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C8">
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="28" priority="35">
       <formula>$C7="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>$C7="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>$C7="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="25" priority="38">
       <formula>$C7="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="13" priority="21">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>$I9="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="23" priority="30">
       <formula>$C9="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="18">
+    <cfRule type="expression" dxfId="22" priority="31">
       <formula>$C9="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="19">
+    <cfRule type="expression" dxfId="21" priority="32">
       <formula>$C9="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="20">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>$C9="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>$C2="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="18" priority="27">
       <formula>$C2="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="17" priority="28">
       <formula>$C2="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="16" priority="29">
       <formula>$C2="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$I10="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="14" priority="14">
+      <formula>$C10="中"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>$C10="低"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>$C10="超高"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="17">
+      <formula>$C10="高"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I12">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>$I11="遅れ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>$C11="中"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>$C11="低"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11">
+      <formula>$C11="超高"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12">
+      <formula>$C11="高"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="expression" dxfId="5" priority="57">
+      <formula>$G22="遅れ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C125">
+    <cfRule type="expression" dxfId="4" priority="67">
+      <formula>$C125="遅れ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$C10="中"</formula>
+      <formula>$C12="中"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$C10="低"</formula>
+      <formula>$C12="低"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$C10="超高"</formula>
+      <formula>$C12="超高"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$C10="高"</formula>
+      <formula>$C12="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1763,7 +2710,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J11 J13:J1048576</xm:sqref>
+          <xm:sqref>J14:J1048576 J1:J12</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Creation  d'un debut de CRUD Mysql
</commit_message>
<xml_diff>
--- a/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
+++ b/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77789E7-F507-407F-9F38-80D0BABE52FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F2208D-6713-4183-8B8F-82209C329E7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{1E56176C-5C6E-4D46-B358-12925D1648B7}"/>
   </bookViews>
@@ -1737,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D38343-8F70-402C-9913-C6A4103E4390}">
   <dimension ref="A1:R130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="I3" s="24" t="str">
         <f t="shared" ref="I3:I10" ca="1" si="0">IF(H3-NOW()&lt;=0,"遅れ",ROUNDDOWN(H3+1-NOW(),0)&amp;"j")</f>
-        <v>5j</v>
+        <v>3j</v>
       </c>
       <c r="J3" s="19">
         <v>0.6</v>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="I4" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5j</v>
+        <v>3j</v>
       </c>
       <c r="J4" s="16">
         <v>0.2</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="I5" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26j</v>
+        <v>24j</v>
       </c>
       <c r="J5" s="16">
         <v>0.12</v>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26j</v>
+        <v>24j</v>
       </c>
       <c r="J6" s="16">
         <v>0</v>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="I7" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26j</v>
+        <v>24j</v>
       </c>
       <c r="J7" s="16">
         <v>0</v>
@@ -2011,7 +2011,7 @@
       </c>
       <c r="I8" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26j</v>
+        <v>24j</v>
       </c>
       <c r="J8" s="16">
         <v>0.6</v>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="I9" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2j</v>
+        <v>遅れ</v>
       </c>
       <c r="J9" s="16">
         <v>0</v>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="I10" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>56j</v>
+        <v>54j</v>
       </c>
       <c r="J10" s="16">
         <v>0</v>

</xml_diff>

<commit_message>
Creation d'un systeme de tracking
Rajotuer un systeme pour recup les infos comme analytics
</commit_message>
<xml_diff>
--- a/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
+++ b/Cahier des charges/Nouveau fichier d'orga travail pers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F2208D-6713-4183-8B8F-82209C329E7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53EDC40-856C-4BD7-B9B4-DC593E46836F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{1E56176C-5C6E-4D46-B358-12925D1648B7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="対応中" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">対応中!$C$1:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">対応中!$C$1:$C$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>No.</t>
   </si>
@@ -194,55 +194,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>今日</t>
-    <rPh sb="0" eb="2">
-      <t>キョウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Creer le generateur de model une fois L'apprentissage termine</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>1) Apprendre a utiliser git ignore
-2) Apprendre a utiliser le Async
-3) Gerrer le proxy
-4) le commit modif
-5) rendre beau le code 
-6) Apprendre comment utiliser les quelques fonctions que je connais pas dans git
-7) Faire en sorte que le check de diagnosis est bie nfait</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>views</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>newUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>updateUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deleteUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>searchUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>adminConnection</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>collection</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Users</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -251,70 +202,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>age</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>address</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>first name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>inscription date</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>mail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>country</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>company</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>job</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>salary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UsersDetail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Users Details</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>viewDetailsUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Model</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UOW</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -476,43 +363,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>明日</t>
-    <rPh sb="0" eb="2">
-      <t>アシタ</t>
-    </rPh>
+    <t>Nodejs project</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Creation d'une application node js SSL socket.io chat Avance. Creation d'une room, message prive, Liste envoie message par radio box</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>1) ok
-2) ok
-3) ok
-4) ok
-5) ok
-6) NON A faire ce soir ou dans le train
-7) A verif demain mais ca a l'air ok
-Ne pas oublier de changer le nom de check ou plutot donner une proposition</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1) Faire le 7)
-2) si 6 pas fait faire le 6
-3) Comprendre le doc de spice et voir un peu ce qu'est ce DCS
-4) Modif le code pour avoir juste les infos necessaires 
-5) Chercher pour check result le comment ca marche
-6) Finir le CRUD Mysql AU MOINS
-7) Si temps finir aussi le CRUD Mongo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8h</t>
-    <phoneticPr fontId="1"/>
+    <t>Creation de agar io</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Creation de generateur de model moongose</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Creation de generateur de model mysql</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>api_rest tracking PM2 test perfo open</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,15 +444,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="0"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -586,7 +456,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,18 +489,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -792,21 +656,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -876,19 +725,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -921,7 +757,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -976,31 +812,19 @@
     <xf numFmtId="9" fontId="6" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1012,16 +836,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1030,49 +848,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1080,7 +889,93 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{B9F7C401-71ED-4AD8-8EED-9CF337C7F41D}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1735,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D38343-8F70-402C-9913-C6A4103E4390}">
-  <dimension ref="A1:R130"/>
+  <dimension ref="A1:R126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1799,17 +1694,17 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:13" ht="276" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="34">
+      <c r="A3" s="28">
         <f>COUNTA(G$3:G3)</f>
         <v>1</v>
       </c>
@@ -1819,30 +1714,30 @@
       <c r="C3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="20">
         <v>43610</v>
       </c>
-      <c r="I3" s="24" t="str">
-        <f t="shared" ref="I3:I10" ca="1" si="0">IF(H3-NOW()&lt;=0,"遅れ",ROUNDDOWN(H3+1-NOW(),0)&amp;"j")</f>
-        <v>3j</v>
+      <c r="I3" s="21" t="str">
+        <f t="shared" ref="I3:I9" ca="1" si="0">IF(H3-NOW()&lt;=0,"遅れ",ROUNDDOWN(H3+1-NOW(),0)&amp;"j")</f>
+        <v>遅れ</v>
       </c>
       <c r="J3" s="19">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="K3" s="18"/>
-      <c r="L3" s="30"/>
+      <c r="L3" s="26"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
@@ -1856,13 +1751,13 @@
       <c r="C4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -1873,13 +1768,13 @@
       </c>
       <c r="I4" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3j</v>
+        <v>遅れ</v>
       </c>
       <c r="J4" s="16">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K4" s="11"/>
-      <c r="L4" s="31"/>
+      <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:13" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A5" s="10">
@@ -1892,13 +1787,13 @@
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -1909,13 +1804,13 @@
       </c>
       <c r="I5" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24j</v>
+        <v>11j</v>
       </c>
       <c r="J5" s="16">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="11"/>
-      <c r="L5" s="31"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
@@ -1928,13 +1823,13 @@
       <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="22" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
@@ -1943,13 +1838,13 @@
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24j</v>
+        <v>11j</v>
       </c>
       <c r="J6" s="16">
         <v>0</v>
       </c>
       <c r="K6" s="11"/>
-      <c r="L6" s="31"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A7" s="10">
@@ -1962,13 +1857,13 @@
       <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13" t="s">
         <v>11</v>
       </c>
@@ -1977,13 +1872,13 @@
       </c>
       <c r="I7" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24j</v>
+        <v>11j</v>
       </c>
       <c r="J7" s="16">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="11"/>
-      <c r="L7" s="31"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A8" s="10">
@@ -1996,11 +1891,11 @@
       <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="22" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -2011,13 +1906,13 @@
       </c>
       <c r="I8" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24j</v>
+        <v>11j</v>
       </c>
       <c r="J8" s="16">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="K8" s="11"/>
-      <c r="L8" s="31"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A9" s="10">
@@ -2036,7 +1931,7 @@
       <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="23" t="s">
         <v>29</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -2050,467 +1945,506 @@
         <v>遅れ</v>
       </c>
       <c r="J9" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="11"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A10" s="10">
-        <f>COUNTA(G$3:G10)</f>
-        <v>8</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="14">
-        <v>43661</v>
-      </c>
-      <c r="I10" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>54j</v>
-      </c>
-      <c r="J10" s="16">
-        <v>0</v>
-      </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A11" s="10">
         <f>COUNTA(G$3:G11)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>36</v>
+      <c r="C11" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="27" t="s">
-        <v>117</v>
+        <v>91</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="14">
-        <v>43605</v>
-      </c>
-      <c r="I11" s="15"/>
+        <v>43661</v>
+      </c>
+      <c r="I11" s="15" t="str">
+        <f t="shared" ref="I11" ca="1" si="1">IF(H11-NOW()&lt;=0,"遅れ",ROUNDDOWN(H11+1-NOW(),0)&amp;"j")</f>
+        <v>41j</v>
+      </c>
       <c r="J11" s="16">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="K11" s="11"/>
-      <c r="L11" s="31"/>
-    </row>
-    <row r="12" spans="1:13" ht="188.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="25">
-        <v>43606</v>
-      </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22">
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="10">
+        <f>COUNTA(G$3:G12)</f>
+        <v>9</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="14">
+        <v>43692</v>
+      </c>
+      <c r="I12" s="15" t="str">
+        <f t="shared" ref="I12:I14" ca="1" si="2">IF(H12-NOW()&lt;=0,"遅れ",ROUNDDOWN(H12+1-NOW(),0)&amp;"j")</f>
+        <v>72j</v>
+      </c>
+      <c r="J12" s="16">
         <v>0</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="32"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="J13" s="7"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="10">
+        <f>COUNTA(G$3:G13)</f>
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="14">
+        <v>43661</v>
+      </c>
+      <c r="I13" s="15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>41j</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="10">
+        <f>COUNTA(G$3:G14)</f>
+        <v>11</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="14">
+        <v>43661</v>
+      </c>
+      <c r="I14" s="15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>41j</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="10">
+        <f>COUNTA(G$3:G15)</f>
+        <v>12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="14">
+        <v>43631</v>
+      </c>
+      <c r="I15" s="15" t="str">
+        <f t="shared" ref="I15" ca="1" si="3">IF(H15-NOW()&lt;=0,"遅れ",ROUNDDOWN(H15+1-NOW(),0)&amp;"j")</f>
+        <v>11j</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="G16" s="7" t="s">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I20" s="7"/>
+      <c r="J20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="9:10" x14ac:dyDescent="0.4">
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="9:18" x14ac:dyDescent="0.4">
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="9:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="9:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I35" s="7"/>
+      <c r="Q35" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="R35" s="39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="9:18" x14ac:dyDescent="0.4">
+      <c r="I36" s="7"/>
+      <c r="Q36" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="R36" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="9:18" x14ac:dyDescent="0.4">
+      <c r="Q37" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="R37" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q38" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="R38" s="33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="H17" s="7" t="s">
+    <row r="39" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q39" s="32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="H18" s="7" t="s">
+      <c r="R39" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="9:18" x14ac:dyDescent="0.4">
+      <c r="Q40" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="R40" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q41" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="R41" s="33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q42" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="R42" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="9:18" ht="60" x14ac:dyDescent="0.4">
+      <c r="Q43" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="R43" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="9:18" x14ac:dyDescent="0.4">
+      <c r="Q44" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="R44" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q45" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="R45" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q46" s="32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="G22" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="E23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="F29" s="7" t="s">
+      <c r="R46" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="H30" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="H31" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="H32" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="H33" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="H34" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="E37" s="7" t="s">
+    </row>
+    <row r="47" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q47" s="32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="5:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="F38" s="7" t="s">
+      <c r="R47" s="33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="5:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="Q39" s="49" t="s">
+    <row r="48" spans="9:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q48" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="R39" s="50" t="s">
+      <c r="R48" s="33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="Q40" s="47" t="s">
+    <row r="49" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q49" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="R40" s="48" t="s">
+      <c r="R49" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="Q41" s="43" t="s">
+    <row r="50" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q50" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="R41" s="44" t="s">
+      <c r="R50" s="33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="5:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q42" s="43" t="s">
+    <row r="51" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q51" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="R42" s="44" t="s">
+      <c r="R51" s="33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="5:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q43" s="43" t="s">
+    <row r="52" spans="17:18" ht="90" x14ac:dyDescent="0.4">
+      <c r="Q52" s="43"/>
+      <c r="R52" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="R43" s="44" t="s">
+    </row>
+    <row r="53" spans="17:18" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q53" s="32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="Q44" s="43" t="s">
+      <c r="R53" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R44" s="44" t="s">
+    </row>
+    <row r="54" spans="17:18" x14ac:dyDescent="0.4">
+      <c r="Q54" s="32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="5:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q45" s="43" t="s">
+      <c r="R54" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="R45" s="44" t="s">
+    </row>
+    <row r="55" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q55" s="32" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="46" spans="5:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q46" s="43" t="s">
+      <c r="R55" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="R46" s="44" t="s">
+    </row>
+    <row r="56" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q56" s="32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="5:18" ht="60" x14ac:dyDescent="0.4">
-      <c r="Q47" s="43" t="s">
+      <c r="R56" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="R47" s="44" t="s">
+    </row>
+    <row r="57" spans="17:18" ht="45" x14ac:dyDescent="0.4">
+      <c r="Q57" s="32" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="48" spans="5:18" x14ac:dyDescent="0.4">
-      <c r="Q48" s="43" t="s">
+      <c r="R57" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="R48" s="44" t="s">
+    </row>
+    <row r="58" spans="17:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="Q58" s="34" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q49" s="43" t="s">
+      <c r="R58" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="R49" s="44" t="s">
+    </row>
+    <row r="99" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J99" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="C121" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="D122" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q50" s="43" t="s">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="D123" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="R50" s="44" t="s">
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="D124" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q51" s="43" t="s">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="E125" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="R51" s="44" t="s">
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="F126" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q52" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="R52" s="44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q53" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="R53" s="44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="17:18" ht="45" x14ac:dyDescent="0.4">
-      <c r="Q54" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="R54" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="17:18" ht="45" x14ac:dyDescent="0.4">
-      <c r="Q55" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="R55" s="44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="17:18" ht="90" x14ac:dyDescent="0.4">
-      <c r="Q56" s="54"/>
-      <c r="R56" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="17:18" ht="30" x14ac:dyDescent="0.4">
-      <c r="Q57" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="R57" s="44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="17:18" x14ac:dyDescent="0.4">
-      <c r="Q58" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="R58" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="17:18" ht="45" x14ac:dyDescent="0.4">
-      <c r="Q59" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="R59" s="44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="17:18" ht="45" x14ac:dyDescent="0.4">
-      <c r="Q60" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="R60" s="44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="61" spans="17:18" ht="45" x14ac:dyDescent="0.4">
-      <c r="Q61" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="R61" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="17:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="Q62" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="R62" s="46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="103" spans="10:10" x14ac:dyDescent="0.4">
-      <c r="J103" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C125" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="D126" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="D127" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="D128" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E129" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="F130" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:C12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:C9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="Q55:Q56"/>
+    <mergeCell ref="Q51:Q52"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="C1 C13:C124 C126:C1048576">
-    <cfRule type="expression" dxfId="39" priority="51">
+  <conditionalFormatting sqref="C1 C16:C120 C10 C122:C1048576">
+    <cfRule type="expression" dxfId="49" priority="86">
       <formula>$C1="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="52">
+    <cfRule type="expression" dxfId="48" priority="87">
       <formula>$C1="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="53">
+    <cfRule type="expression" dxfId="47" priority="88">
       <formula>$C1="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="54">
+    <cfRule type="expression" dxfId="46" priority="89">
       <formula>$C1="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="dataBar" priority="50">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -2523,13 +2457,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I2 I24:I123 I13:I22 I125:I1048576">
-    <cfRule type="expression" dxfId="35" priority="45">
+  <conditionalFormatting sqref="I1:I2 I37:I119 I10 I121:I1048576">
+    <cfRule type="expression" dxfId="45" priority="80">
       <formula>$I1="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J1048576 J1:J12">
-    <cfRule type="dataBar" priority="55">
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -2543,136 +2477,174 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="expression" dxfId="34" priority="41">
+    <cfRule type="expression" dxfId="44" priority="76">
       <formula>$C3="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="42">
+    <cfRule type="expression" dxfId="43" priority="77">
       <formula>$C3="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="42" priority="78">
       <formula>$C3="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="44">
+    <cfRule type="expression" dxfId="41" priority="79">
       <formula>$C3="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I6">
-    <cfRule type="expression" dxfId="30" priority="40">
+    <cfRule type="expression" dxfId="40" priority="75">
       <formula>$I3="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I8">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="39" priority="74">
       <formula>$I7="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C8">
-    <cfRule type="expression" dxfId="28" priority="35">
+    <cfRule type="expression" dxfId="38" priority="70">
       <formula>$C7="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="36">
+    <cfRule type="expression" dxfId="37" priority="71">
       <formula>$C7="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="37">
+    <cfRule type="expression" dxfId="36" priority="72">
       <formula>$C7="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="38">
+    <cfRule type="expression" dxfId="35" priority="73">
       <formula>$C7="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="24" priority="34">
+    <cfRule type="expression" dxfId="34" priority="69">
       <formula>$I9="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="33" priority="65">
       <formula>$C9="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="32" priority="66">
       <formula>$C9="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="32">
+    <cfRule type="expression" dxfId="31" priority="67">
       <formula>$C9="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="33">
+    <cfRule type="expression" dxfId="30" priority="68">
       <formula>$C9="高"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="19" priority="26">
+    <cfRule type="expression" dxfId="29" priority="61">
       <formula>$C2="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="27">
+    <cfRule type="expression" dxfId="28" priority="62">
       <formula>$C2="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="28">
+    <cfRule type="expression" dxfId="27" priority="63">
       <formula>$C2="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="29">
+    <cfRule type="expression" dxfId="26" priority="64">
       <formula>$C2="高"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="15" priority="18">
-      <formula>$I10="遅れ"</formula>
+  <conditionalFormatting sqref="C121">
+    <cfRule type="expression" dxfId="25" priority="102">
+      <formula>$C121="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>$C10="中"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>$C10="低"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>$C10="超高"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="17">
-      <formula>$C10="高"</formula>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="24" priority="6">
+      <formula>$C14="中"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="7">
+      <formula>$C14="低"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="8">
+      <formula>$C14="超高"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="9">
+      <formula>$C14="高"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I12">
-    <cfRule type="expression" dxfId="10" priority="13">
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="20" priority="35">
       <formula>$I11="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="19" priority="31">
       <formula>$C11="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="18" priority="32">
       <formula>$C11="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="17" priority="33">
       <formula>$C11="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="16" priority="34">
       <formula>$C11="高"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="expression" dxfId="5" priority="57">
-      <formula>$G22="遅れ"</formula>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="15" priority="10">
+      <formula>$I14="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C125">
-    <cfRule type="expression" dxfId="4" priority="67">
-      <formula>$C125="遅れ"</formula>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="14" priority="25">
+      <formula>$I12="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="13" priority="21">
       <formula>$C12="中"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="12" priority="22">
       <formula>$C12="低"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>$C12="超高"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="10" priority="24">
       <formula>$C12="高"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>$I13="遅れ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>$C13="中"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="12">
+      <formula>$C13="低"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>$C13="超高"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="14">
+      <formula>$C13="高"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$C15="中"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$C15="低"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$C15="超高"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>$C15="高"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>$I15="遅れ"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2710,7 +2682,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J14:J1048576 J1:J12</xm:sqref>
+          <xm:sqref>J1:J1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>